<commit_message>
AutoTraderTest files - first test for selecting number of images in the search results
</commit_message>
<xml_diff>
--- a/Testing/Auto-Trader_Testing/lookups.xlsx
+++ b/Testing/Auto-Trader_Testing/lookups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\EclipseWorkSpace\QA-training\Testing\Automated_Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\EclipseWorkSpace\QA-training\Testing\Auto-Trader_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,18 +24,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ffdfs</t>
-  </si>
-  <si>
-    <t>mmmm</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+  <si>
+    <t>PostCode</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>MinPrice</t>
+  </si>
+  <si>
+    <t>MaxPrice</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>cw1 2jb</t>
+  </si>
+  <si>
+    <t>NumberOfSearches</t>
   </si>
 </sst>
 </file>
@@ -71,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,31 +369,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>